<commit_message>
Pushing to git for GenBank submissions
</commit_message>
<xml_diff>
--- a/genbank/SRA_metadata-aquaculture.xlsx
+++ b/genbank/SRA_metadata-aquaculture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/github/lates-wgs/genbank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1756B2FC-F3BF-3E4F-82B6-54BBEFFAF44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB284C9-9142-6241-831E-670976A225C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50880" yWindow="500" windowWidth="37220" windowHeight="24920" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-56920" yWindow="500" windowWidth="37220" windowHeight="24920" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact Info and Instructions" sheetId="3" r:id="rId1"/>
@@ -2190,6 +2190,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="62"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="62" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2202,6 +2203,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2211,10 +2215,6 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="77">
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
@@ -2747,52 +2747,52 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
     </row>
     <row r="7" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
@@ -2852,15 +2852,15 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2892,27 +2892,27 @@
       <c r="B37" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
     </row>
     <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="21" t="s">
@@ -2985,7 +2985,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M41" sqref="M41:M45"/>
+      <selection pane="topRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3061,10 +3061,10 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="36" t="s">
         <v>294</v>
       </c>
       <c r="C2" s="10" t="str">
@@ -3103,10 +3103,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="36" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="36" t="s">
         <v>295</v>
       </c>
       <c r="C3" s="10" t="str">
@@ -3145,10 +3145,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="36" t="s">
         <v>296</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="36" t="s">
         <v>296</v>
       </c>
       <c r="C4" s="10" t="str">
@@ -3187,10 +3187,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="36" t="s">
         <v>297</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="36" t="s">
         <v>297</v>
       </c>
       <c r="C5" s="10" t="str">
@@ -3229,10 +3229,10 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="36" t="s">
         <v>298</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="36" t="s">
         <v>298</v>
       </c>
       <c r="C6" s="10" t="str">
@@ -3271,10 +3271,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="36" t="s">
         <v>299</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="36" t="s">
         <v>299</v>
       </c>
       <c r="C7" s="10" t="str">
@@ -3313,10 +3313,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="36" t="s">
         <v>300</v>
       </c>
       <c r="C8" s="10" t="str">
@@ -3355,10 +3355,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="36" t="s">
         <v>301</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="36" t="s">
         <v>301</v>
       </c>
       <c r="C9" s="10" t="str">
@@ -3397,10 +3397,10 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="36" t="s">
         <v>302</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="36" t="s">
         <v>302</v>
       </c>
       <c r="C10" s="10" t="str">
@@ -3439,10 +3439,10 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="36" t="s">
         <v>303</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="36" t="s">
         <v>303</v>
       </c>
       <c r="C11" s="10" t="str">
@@ -3481,10 +3481,10 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="36" t="s">
         <v>304</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="36" t="s">
         <v>304</v>
       </c>
       <c r="C12" s="10" t="str">
@@ -3523,10 +3523,10 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="36" t="s">
         <v>305</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="36" t="s">
         <v>305</v>
       </c>
       <c r="C13" s="10" t="str">
@@ -3565,10 +3565,10 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="36" t="s">
         <v>306</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="36" t="s">
         <v>306</v>
       </c>
       <c r="C14" s="10" t="str">
@@ -3607,10 +3607,10 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="36" t="s">
         <v>307</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="36" t="s">
         <v>307</v>
       </c>
       <c r="C15" s="10" t="str">
@@ -3649,10 +3649,10 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="36" t="s">
         <v>308</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="36" t="s">
         <v>308</v>
       </c>
       <c r="C16" s="10" t="str">
@@ -3691,10 +3691,10 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="36" t="s">
         <v>309</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="36" t="s">
         <v>309</v>
       </c>
       <c r="C17" s="10" t="str">
@@ -3733,10 +3733,10 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="36" t="s">
         <v>310</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="36" t="s">
         <v>310</v>
       </c>
       <c r="C18" s="10" t="str">
@@ -3775,10 +3775,10 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="36" t="s">
         <v>311</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="36" t="s">
         <v>311</v>
       </c>
       <c r="C19" s="10" t="str">
@@ -3817,10 +3817,10 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="36" t="s">
         <v>312</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="36" t="s">
         <v>312</v>
       </c>
       <c r="C20" s="10" t="str">
@@ -3859,10 +3859,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="36" t="s">
         <v>313</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="36" t="s">
         <v>313</v>
       </c>
       <c r="C21" s="10" t="str">
@@ -3901,10 +3901,10 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="36" t="s">
         <v>314</v>
       </c>
       <c r="C22" s="10" t="str">
@@ -3943,10 +3943,10 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="36" t="s">
         <v>315</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="36" t="s">
         <v>315</v>
       </c>
       <c r="C23" s="10" t="str">
@@ -3985,10 +3985,10 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="36" t="s">
         <v>316</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="36" t="s">
         <v>316</v>
       </c>
       <c r="C24" s="10" t="str">
@@ -4027,10 +4027,10 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="36" t="s">
         <v>317</v>
       </c>
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="36" t="s">
         <v>317</v>
       </c>
       <c r="C25" s="10" t="str">
@@ -4069,10 +4069,10 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="36" t="s">
         <v>318</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="36" t="s">
         <v>318</v>
       </c>
       <c r="C26" s="10" t="str">
@@ -4111,10 +4111,10 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="36" t="s">
         <v>319</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="36" t="s">
         <v>319</v>
       </c>
       <c r="C27" s="10" t="str">
@@ -4153,10 +4153,10 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="36" t="s">
         <v>320</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="36" t="s">
         <v>320</v>
       </c>
       <c r="C28" s="10" t="str">
@@ -4195,10 +4195,10 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="36" t="s">
         <v>321</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="36" t="s">
         <v>321</v>
       </c>
       <c r="C29" s="10" t="str">
@@ -4237,10 +4237,10 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="36" t="s">
         <v>322</v>
       </c>
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="36" t="s">
         <v>322</v>
       </c>
       <c r="C30" s="10" t="str">
@@ -4279,10 +4279,10 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="36" t="s">
         <v>323</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="36" t="s">
         <v>323</v>
       </c>
       <c r="C31" s="10" t="str">
@@ -4321,10 +4321,10 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="36" t="s">
         <v>324</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="36" t="s">
         <v>324</v>
       </c>
       <c r="C32" s="10" t="str">
@@ -4363,10 +4363,10 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="36" t="s">
         <v>325</v>
       </c>
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="36" t="s">
         <v>325</v>
       </c>
       <c r="C33" s="10" t="str">
@@ -4405,10 +4405,10 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="36" t="s">
         <v>326</v>
       </c>
-      <c r="B34" s="46" t="s">
+      <c r="B34" s="36" t="s">
         <v>326</v>
       </c>
       <c r="C34" s="10" t="str">
@@ -4447,10 +4447,10 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="36" t="s">
         <v>327</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="36" t="s">
         <v>327</v>
       </c>
       <c r="C35" s="10" t="str">
@@ -4489,10 +4489,10 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="36" t="s">
         <v>328</v>
       </c>
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="36" t="s">
         <v>328</v>
       </c>
       <c r="C36" s="10" t="str">
@@ -4531,10 +4531,10 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="36" t="s">
         <v>329</v>
       </c>
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="36" t="s">
         <v>329</v>
       </c>
       <c r="C37" s="10" t="str">
@@ -4573,10 +4573,10 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="36" t="s">
         <v>330</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="36" t="s">
         <v>330</v>
       </c>
       <c r="C38" s="10" t="str">
@@ -4615,10 +4615,10 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="36" t="s">
         <v>331</v>
       </c>
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="36" t="s">
         <v>331</v>
       </c>
       <c r="C39" s="10" t="str">
@@ -4657,10 +4657,10 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="36" t="s">
         <v>332</v>
       </c>
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="36" t="s">
         <v>332</v>
       </c>
       <c r="C40" s="10" t="str">
@@ -4699,10 +4699,10 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="36" t="s">
         <v>333</v>
       </c>
-      <c r="B41" s="46" t="s">
+      <c r="B41" s="36" t="s">
         <v>333</v>
       </c>
       <c r="C41" s="10" t="str">
@@ -4741,10 +4741,10 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="36" t="s">
         <v>334</v>
       </c>
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="36" t="s">
         <v>334</v>
       </c>
       <c r="C42" s="10" t="str">
@@ -4783,10 +4783,10 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="36" t="s">
         <v>335</v>
       </c>
-      <c r="B43" s="46" t="s">
+      <c r="B43" s="36" t="s">
         <v>335</v>
       </c>
       <c r="C43" s="10" t="str">
@@ -4825,10 +4825,10 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="36" t="s">
         <v>336</v>
       </c>
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="36" t="s">
         <v>336</v>
       </c>
       <c r="C44" s="10" t="str">
@@ -4867,10 +4867,10 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="46" t="s">
+      <c r="A45" s="36" t="s">
         <v>337</v>
       </c>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="36" t="s">
         <v>337</v>
       </c>
       <c r="C45" s="10" t="str">
@@ -7149,15 +7149,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
     </row>
     <row r="2" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="45"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -7169,172 +7169,172 @@
       <c r="A3" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="41"/>
+      <c r="C3" s="42"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="41"/>
+      <c r="C4" s="42"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="42"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="42"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="41"/>
+      <c r="C7" s="42"/>
     </row>
     <row r="8" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="41"/>
+      <c r="C8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="41"/>
+      <c r="C9" s="42"/>
     </row>
     <row r="10" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="41"/>
+      <c r="C10" s="42"/>
     </row>
     <row r="11" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="42"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="41"/>
+      <c r="C12" s="42"/>
     </row>
     <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="41"/>
+      <c r="C13" s="42"/>
     </row>
     <row r="14" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="41"/>
+      <c r="C14" s="42"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="41"/>
+      <c r="C15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="41"/>
+      <c r="C16" s="42"/>
     </row>
     <row r="17" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="41"/>
+      <c r="C17" s="42"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="41"/>
+      <c r="C18" s="42"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="41"/>
+      <c r="C19" s="42"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="41"/>
+      <c r="C20" s="42"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="C21" s="41"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -7346,28 +7346,28 @@
       <c r="A22" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="41"/>
+      <c r="C22" s="42"/>
     </row>
     <row r="23" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="41"/>
+      <c r="C23" s="42"/>
     </row>
     <row r="24" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="41"/>
+      <c r="C24" s="42"/>
     </row>
     <row r="25" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
@@ -7471,10 +7471,10 @@
       <c r="A37" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="46" t="s">
         <v>284</v>
       </c>
-      <c r="C37" s="44"/>
+      <c r="C37" s="46"/>
       <c r="D37" s="34"/>
       <c r="E37" s="34"/>
       <c r="F37" s="34"/>
@@ -7519,11 +7519,11 @@
       <c r="A42" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B42" s="44" t="s">
+      <c r="B42" s="46" t="s">
         <v>290</v>
       </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
       <c r="E42" s="34"/>
       <c r="F42" s="34"/>
       <c r="G42" s="34"/>
@@ -7534,75 +7534,75 @@
       <c r="A43" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="C43" s="41"/>
+      <c r="C43" s="42"/>
     </row>
     <row r="44" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
     </row>
     <row r="45" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="42"/>
-      <c r="C45" s="43"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="45"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="C46" s="41"/>
+      <c r="C46" s="42"/>
     </row>
     <row r="47" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="41"/>
+      <c r="C47" s="42"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="C48" s="41"/>
+      <c r="C48" s="42"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="C49" s="41"/>
+      <c r="C49" s="42"/>
     </row>
     <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="C50" s="41"/>
+      <c r="C50" s="42"/>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B51" s="41" t="s">
+      <c r="B51" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="C51" s="41"/>
+      <c r="C51" s="42"/>
     </row>
     <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
@@ -7618,264 +7618,264 @@
       <c r="A54" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="C54" s="41"/>
+      <c r="C54" s="42"/>
     </row>
     <row r="55" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
     </row>
     <row r="56" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="41"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="42"/>
     </row>
     <row r="57" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="C57" s="41"/>
+      <c r="C57" s="42"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="41" t="s">
+      <c r="B58" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="C58" s="41"/>
+      <c r="C58" s="42"/>
     </row>
     <row r="59" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="C59" s="41"/>
+      <c r="C59" s="42"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B60" s="41" t="s">
+      <c r="B60" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="C60" s="41"/>
+      <c r="C60" s="42"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="41" t="s">
+      <c r="B61" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="C61" s="41"/>
+      <c r="C61" s="42"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B62" s="41" t="s">
+      <c r="B62" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="C62" s="41"/>
+      <c r="C62" s="42"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B63" s="41" t="s">
+      <c r="B63" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="C63" s="41"/>
+      <c r="C63" s="42"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B64" s="41" t="s">
+      <c r="B64" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="C64" s="41"/>
+      <c r="C64" s="42"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="C65" s="41"/>
+      <c r="C65" s="42"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="41" t="s">
+      <c r="B66" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="C66" s="41"/>
+      <c r="C66" s="42"/>
     </row>
     <row r="67" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B67" s="41" t="s">
+      <c r="B67" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="C67" s="41"/>
+      <c r="C67" s="42"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B68" s="41" t="s">
+      <c r="B68" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="C68" s="41"/>
+      <c r="C68" s="42"/>
     </row>
     <row r="69" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B69" s="41" t="s">
+      <c r="B69" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="C69" s="41"/>
+      <c r="C69" s="42"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="B70" s="41" t="s">
+      <c r="B70" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="C70" s="41"/>
+      <c r="C70" s="42"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B71" s="41" t="s">
+      <c r="B71" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="C71" s="41"/>
+      <c r="C71" s="42"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B72" s="41" t="s">
+      <c r="B72" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="C72" s="41"/>
+      <c r="C72" s="42"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B73" s="41" t="s">
+      <c r="B73" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="C73" s="41"/>
+      <c r="C73" s="42"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B74" s="41" t="s">
+      <c r="B74" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="C74" s="41"/>
+      <c r="C74" s="42"/>
     </row>
     <row r="75" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="B75" s="41" t="s">
+      <c r="B75" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="C75" s="41"/>
+      <c r="C75" s="42"/>
     </row>
     <row r="76" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B76" s="41" t="s">
+      <c r="B76" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="41"/>
+      <c r="C76" s="42"/>
     </row>
     <row r="77" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="B77" s="41" t="s">
+      <c r="B77" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="41"/>
+      <c r="C77" s="42"/>
     </row>
     <row r="78" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B78" s="41" t="s">
+      <c r="B78" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="C78" s="41"/>
+      <c r="C78" s="42"/>
     </row>
     <row r="79" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B79" s="41" t="s">
+      <c r="B79" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="C79" s="41"/>
+      <c r="C79" s="42"/>
     </row>
     <row r="80" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B80" s="41" t="s">
+      <c r="B80" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="C80" s="41"/>
+      <c r="C80" s="42"/>
     </row>
     <row r="81" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B81" s="41" t="s">
+      <c r="B81" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="C81" s="41"/>
+      <c r="C81" s="42"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A82" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B82" s="41" t="s">
+      <c r="B82" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="C82" s="41"/>
+      <c r="C82" s="42"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A83" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="41" t="s">
+      <c r="B83" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="C83" s="41"/>
+      <c r="C83" s="42"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A84" s="2" t="s">
@@ -8329,40 +8329,25 @@
     <sortCondition ref="J93"/>
   </sortState>
   <mergeCells count="65">
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
@@ -8375,25 +8360,40 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>